<commit_message>
R2 cambiado, makefile mejorado y cambios en el excel
</commit_message>
<xml_diff>
--- a/seed-src/Reuniones de seguimiento y Cronograma/Cronograma I3 Grupo B.xlsx
+++ b/seed-src/Reuniones de seguimiento y Cronograma/Cronograma I3 Grupo B.xlsx
@@ -241,7 +241,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-C0A];[RED]\-#,##0.00\ [$€-C0A]"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -450,6 +450,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <i val="true"/>
       <sz val="11"/>
@@ -459,7 +467,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,7 +501,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -536,6 +544,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFCC0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -694,7 +708,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -755,7 +769,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="14" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -779,62 +793,62 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="14" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="15" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="15" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="10" borderId="4" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="4" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="4" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="10" borderId="4" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="16" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="12" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="12" borderId="4" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="14" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="10" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="10" borderId="4" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="4" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="4" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="10" borderId="4" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="15" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="12" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="12" borderId="4" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="34" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -863,11 +877,11 @@
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="15" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="16" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="15" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="16" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -879,12 +893,16 @@
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="16" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="17" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="26" fillId="10" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="25" fillId="10" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -903,15 +921,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="15" borderId="4" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="16" borderId="4" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -919,15 +937,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -966,13 +984,13 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF996600"/>
@@ -1032,8 +1050,8 @@
   </sheetPr>
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F4" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X28" activeCellId="0" sqref="X28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1303,7 +1321,7 @@
       <c r="B8" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="16"/>
@@ -1335,7 +1353,7 @@
       <c r="B9" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="21" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="16"/>
@@ -1367,7 +1385,7 @@
       <c r="B10" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="16"/>
@@ -1399,7 +1417,7 @@
       <c r="B11" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="16"/>
@@ -1431,7 +1449,7 @@
       <c r="B12" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="16"/>
@@ -1463,7 +1481,7 @@
       <c r="B13" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="21" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="16"/>
@@ -1985,14 +2003,14 @@
         <v>14</v>
       </c>
       <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="G29" s="48"/>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
       <c r="J29" s="24"/>
       <c r="K29" s="18"/>
       <c r="L29" s="26"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="48"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
       <c r="O29" s="24"/>
       <c r="P29" s="24"/>
       <c r="Q29" s="24"/>
@@ -2092,7 +2110,7 @@
       <c r="Q32" s="14"/>
       <c r="R32" s="14"/>
       <c r="S32" s="14"/>
-      <c r="T32" s="49"/>
+      <c r="T32" s="50"/>
       <c r="U32" s="14"/>
       <c r="V32" s="14"/>
     </row>
@@ -2135,7 +2153,7 @@
       <c r="B34" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="21" t="s">
         <v>54</v>
       </c>
       <c r="D34" s="16" t="s">
@@ -2150,13 +2168,13 @@
       <c r="G34" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="50"/>
+      <c r="H34" s="51"/>
       <c r="I34" s="24"/>
       <c r="J34" s="24"/>
       <c r="K34" s="24"/>
       <c r="L34" s="23"/>
       <c r="M34" s="19"/>
-      <c r="N34" s="51"/>
+      <c r="N34" s="52"/>
       <c r="O34" s="19"/>
       <c r="P34" s="19"/>
       <c r="Q34" s="19"/>
@@ -2199,9 +2217,9 @@
       <c r="P35" s="19"/>
       <c r="Q35" s="19"/>
       <c r="R35" s="18"/>
-      <c r="S35" s="51"/>
-      <c r="T35" s="51"/>
-      <c r="U35" s="51"/>
+      <c r="S35" s="52"/>
+      <c r="T35" s="52"/>
+      <c r="U35" s="52"/>
       <c r="V35" s="46"/>
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2211,7 +2229,7 @@
       <c r="B36" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="21" t="s">
         <v>58</v>
       </c>
       <c r="D36" s="16"/>
@@ -2230,8 +2248,8 @@
       <c r="O36" s="18"/>
       <c r="P36" s="18"/>
       <c r="Q36" s="18"/>
-      <c r="R36" s="52"/>
-      <c r="S36" s="52"/>
+      <c r="R36" s="53"/>
+      <c r="S36" s="53"/>
       <c r="T36" s="31"/>
       <c r="U36" s="18"/>
       <c r="V36" s="14"/>
@@ -2301,9 +2319,9 @@
       <c r="P38" s="19"/>
       <c r="Q38" s="19"/>
       <c r="R38" s="17"/>
-      <c r="S38" s="51"/>
-      <c r="T38" s="51"/>
-      <c r="U38" s="51"/>
+      <c r="S38" s="52"/>
+      <c r="T38" s="52"/>
+      <c r="U38" s="52"/>
       <c r="V38" s="14"/>
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2383,67 +2401,67 @@
       <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="55" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="55" t="s">
+      <c r="B4" s="57"/>
+      <c r="C4" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="55" t="s">
+      <c r="B5" s="58"/>
+      <c r="C5" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="55" t="s">
+      <c r="B6" s="59"/>
+      <c r="C6" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Ya se pueden utilizar varios objetos tanto con el take como con el drop
</commit_message>
<xml_diff>
--- a/seed-src/Reuniones de seguimiento y Cronograma/Cronograma I3 Grupo B.xlsx
+++ b/seed-src/Reuniones de seguimiento y Cronograma/Cronograma I3 Grupo B.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="71">
   <si>
     <t xml:space="preserve">CRONOGRAMA I3</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t xml:space="preserve">Modificar comando take (ya implementado en I2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificar comando drop</t>
   </si>
   <si>
     <t xml:space="preserve">R14</t>
@@ -708,7 +711,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -845,10 +848,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="14" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="34" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -909,7 +908,7 @@
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1048,10 +1047,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X46"/>
+  <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="28:30"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1513,7 +1512,7 @@
       <c r="B14" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="16"/>
@@ -1545,7 +1544,7 @@
       <c r="B15" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="21" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="16"/>
@@ -1577,7 +1576,7 @@
       <c r="B16" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="22" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="16"/>
@@ -1589,8 +1588,8 @@
       <c r="H16" s="23"/>
       <c r="I16" s="29"/>
       <c r="J16" s="28"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="36"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="35"/>
       <c r="M16" s="24"/>
       <c r="N16" s="24"/>
       <c r="O16" s="14"/>
@@ -1609,7 +1608,7 @@
       <c r="B17" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="16"/>
@@ -1635,7 +1634,7 @@
       <c r="V17" s="19"/>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="36" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="14" t="n">
@@ -1651,9 +1650,9 @@
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="28"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
@@ -1665,10 +1664,10 @@
       <c r="T18" s="19"/>
       <c r="U18" s="19"/>
       <c r="V18" s="19"/>
-      <c r="X18" s="39"/>
+      <c r="X18" s="38"/>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="36" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="14" t="n">
@@ -1684,9 +1683,9 @@
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="28"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
@@ -1700,7 +1699,7 @@
       <c r="V19" s="19"/>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="36" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="14" t="n">
@@ -1716,9 +1715,9 @@
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="28"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
       <c r="N20" s="28"/>
@@ -1732,7 +1731,7 @@
       <c r="V20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="36" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="14" t="n">
@@ -1748,9 +1747,9 @@
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="28"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="41"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="40"/>
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
       <c r="N21" s="24"/>
@@ -1764,7 +1763,7 @@
       <c r="V21" s="19"/>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="36" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="14" t="n">
@@ -1780,9 +1779,9 @@
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="28"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="41"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="40"/>
       <c r="L22" s="23"/>
       <c r="M22" s="24"/>
       <c r="N22" s="24"/>
@@ -1796,7 +1795,7 @@
       <c r="V22" s="19"/>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="36" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="14" t="n">
@@ -1812,10 +1811,10 @@
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="24"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="35"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="34"/>
       <c r="M23" s="24"/>
       <c r="N23" s="24"/>
       <c r="O23" s="14"/>
@@ -1848,8 +1847,8 @@
       <c r="J24" s="24"/>
       <c r="K24" s="24"/>
       <c r="L24" s="28"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="43"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="42"/>
       <c r="O24" s="31"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
@@ -1858,6 +1857,7 @@
       <c r="T24" s="14"/>
       <c r="U24" s="19"/>
       <c r="V24" s="19"/>
+      <c r="W24" s="38"/>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="20" t="s">
@@ -1913,9 +1913,9 @@
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
       <c r="M26" s="18"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
-      <c r="P26" s="44"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="18"/>
       <c r="S26" s="18"/>
@@ -1930,7 +1930,7 @@
       <c r="B27" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="21" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="16" t="s">
@@ -1940,9 +1940,9 @@
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
       <c r="H27" s="24"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="45"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
       <c r="L27" s="23"/>
       <c r="M27" s="19"/>
       <c r="N27" s="19"/>
@@ -1959,7 +1959,7 @@
       <c r="A28" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="46" t="n">
+      <c r="B28" s="45" t="n">
         <v>1</v>
       </c>
       <c r="C28" s="15" t="s">
@@ -1976,8 +1976,8 @@
       <c r="J28" s="24"/>
       <c r="K28" s="24"/>
       <c r="L28" s="26"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
       <c r="O28" s="19"/>
       <c r="P28" s="19"/>
       <c r="Q28" s="19"/>
@@ -1986,7 +1986,7 @@
       <c r="T28" s="19"/>
       <c r="U28" s="19"/>
       <c r="V28" s="28"/>
-      <c r="X28" s="39"/>
+      <c r="X28" s="38"/>
     </row>
     <row r="29" customFormat="false" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="25" t="s">
@@ -2003,14 +2003,14 @@
         <v>14</v>
       </c>
       <c r="F29" s="16"/>
-      <c r="G29" s="48"/>
+      <c r="G29" s="47"/>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
       <c r="J29" s="24"/>
       <c r="K29" s="18"/>
       <c r="L29" s="26"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="49"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="48"/>
       <c r="O29" s="24"/>
       <c r="P29" s="24"/>
       <c r="Q29" s="24"/>
@@ -2040,7 +2040,7 @@
       <c r="I30" s="24"/>
       <c r="J30" s="24"/>
       <c r="K30" s="28"/>
-      <c r="L30" s="35"/>
+      <c r="L30" s="34"/>
       <c r="M30" s="24"/>
       <c r="N30" s="24"/>
       <c r="O30" s="25"/>
@@ -2083,7 +2083,7 @@
       <c r="V31" s="14"/>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="36" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="14" t="n">
@@ -2103,26 +2103,26 @@
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="37"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
       <c r="Q32" s="14"/>
       <c r="R32" s="14"/>
       <c r="S32" s="14"/>
-      <c r="T32" s="50"/>
+      <c r="T32" s="49"/>
       <c r="U32" s="14"/>
       <c r="V32" s="14"/>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="37" t="s">
-        <v>51</v>
+      <c r="A33" s="36" t="s">
+        <v>49</v>
       </c>
       <c r="B33" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C33" s="15" t="s">
-        <v>52</v>
+      <c r="C33" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -2130,70 +2130,64 @@
         <v>14</v>
       </c>
       <c r="G33" s="16"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="41"/>
-      <c r="O33" s="41"/>
-      <c r="P33" s="41"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="37"/>
-      <c r="U33" s="18"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="49"/>
+      <c r="U33" s="14"/>
       <c r="V33" s="14"/>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13" t="s">
-        <v>53</v>
+      <c r="A34" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="B34" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C34" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>14</v>
-      </c>
+      <c r="C34" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
       <c r="F34" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="51"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="17"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="40"/>
+      <c r="N34" s="40"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="40"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
       <c r="S34" s="18"/>
-      <c r="T34" s="18"/>
-      <c r="U34" s="17"/>
+      <c r="T34" s="36"/>
+      <c r="U34" s="18"/>
       <c r="V34" s="14"/>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>56</v>
-      </c>
       <c r="D35" s="16" t="s">
         <v>14</v>
       </c>
@@ -2206,108 +2200,108 @@
       <c r="G35" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="24"/>
+      <c r="H35" s="50"/>
       <c r="I35" s="24"/>
       <c r="J35" s="24"/>
       <c r="K35" s="24"/>
       <c r="L35" s="23"/>
       <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
+      <c r="N35" s="51"/>
       <c r="O35" s="19"/>
       <c r="P35" s="19"/>
       <c r="Q35" s="19"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="52"/>
-      <c r="T35" s="52"/>
-      <c r="U35" s="52"/>
-      <c r="V35" s="46"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="18"/>
+      <c r="U35" s="17"/>
+      <c r="V35" s="14"/>
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="21" t="s">
+      <c r="D36" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="51"/>
+      <c r="T36" s="51"/>
+      <c r="U36" s="51"/>
+      <c r="V36" s="45"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="25" t="s">
         <v>58</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="53"/>
-      <c r="S36" s="53"/>
-      <c r="T36" s="31"/>
-      <c r="U36" s="18"/>
-      <c r="V36" s="14"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="20" t="s">
-        <v>59</v>
       </c>
       <c r="B37" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C37" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E37" s="16"/>
+      <c r="C37" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="44"/>
-      <c r="S37" s="44"/>
-      <c r="T37" s="44"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="52"/>
+      <c r="S37" s="52"/>
+      <c r="T37" s="31"/>
       <c r="U37" s="18"/>
       <c r="V37" s="14"/>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>62</v>
-      </c>
       <c r="D38" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>14</v>
-      </c>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
       <c r="H38" s="24"/>
       <c r="I38" s="24"/>
       <c r="J38" s="24"/>
@@ -2318,21 +2312,21 @@
       <c r="O38" s="19"/>
       <c r="P38" s="19"/>
       <c r="Q38" s="19"/>
-      <c r="R38" s="17"/>
-      <c r="S38" s="52"/>
-      <c r="T38" s="52"/>
-      <c r="U38" s="52"/>
+      <c r="R38" s="43"/>
+      <c r="S38" s="43"/>
+      <c r="T38" s="43"/>
+      <c r="U38" s="18"/>
       <c r="V38" s="14"/>
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="B39" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>64</v>
       </c>
       <c r="D39" s="16" t="s">
         <v>14</v>
@@ -2356,19 +2350,57 @@
       <c r="O39" s="19"/>
       <c r="P39" s="19"/>
       <c r="Q39" s="19"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="19"/>
-      <c r="T39" s="19"/>
-      <c r="U39" s="19"/>
-      <c r="V39" s="13"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="51"/>
+      <c r="T39" s="51"/>
+      <c r="U39" s="51"/>
+      <c r="V39" s="14"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="13"/>
+    </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:V1"/>
@@ -2395,73 +2427,73 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="28:30 C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
+      <c r="A1" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Todo lo de links terminado y ademas se ha incluido lo de graphic enginge
</commit_message>
<xml_diff>
--- a/seed-src/Reuniones de seguimiento y Cronograma/Cronograma I3 Grupo B.xlsx
+++ b/seed-src/Reuniones de seguimiento y Cronograma/Cronograma I3 Grupo B.xlsx
@@ -454,15 +454,15 @@
     </font>
     <font>
       <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color rgb="FF999999"/>
       <name val="Times New Roman"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
@@ -892,6 +892,10 @@
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="25" fillId="16" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -920,7 +924,7 @@
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -930,10 +934,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="13" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="25" fillId="13" borderId="3" xfId="34" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1078,7 +1078,7 @@
   <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+      <selection pane="topLeft" activeCell="U23" activeCellId="0" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1851,7 +1851,7 @@
       <c r="R23" s="14"/>
       <c r="S23" s="14"/>
       <c r="T23" s="14"/>
-      <c r="U23" s="19"/>
+      <c r="U23" s="41"/>
       <c r="V23" s="24"/>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1875,8 +1875,8 @@
       <c r="J24" s="24"/>
       <c r="K24" s="24"/>
       <c r="L24" s="28"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="43"/>
       <c r="O24" s="31"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
@@ -1894,7 +1894,7 @@
       <c r="B25" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="16" t="s">
@@ -1926,7 +1926,7 @@
       <c r="B26" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="21" t="s">
         <v>39</v>
       </c>
       <c r="D26" s="16" t="s">
@@ -1941,9 +1941,9 @@
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
       <c r="M26" s="18"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="44"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="18"/>
       <c r="S26" s="18"/>
@@ -1968,9 +1968,9 @@
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
       <c r="H27" s="24"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
       <c r="L27" s="23"/>
       <c r="M27" s="19"/>
       <c r="N27" s="19"/>
@@ -1987,7 +1987,7 @@
       <c r="A28" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="45" t="n">
+      <c r="B28" s="46" t="n">
         <v>1</v>
       </c>
       <c r="C28" s="21" t="s">
@@ -2004,8 +2004,8 @@
       <c r="J28" s="24"/>
       <c r="K28" s="24"/>
       <c r="L28" s="26"/>
-      <c r="M28" s="46"/>
-      <c r="N28" s="46"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="47"/>
       <c r="O28" s="19"/>
       <c r="P28" s="19"/>
       <c r="Q28" s="19"/>
@@ -2023,7 +2023,7 @@
       <c r="B29" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="48" t="s">
         <v>44</v>
       </c>
       <c r="D29" s="16"/>
@@ -2031,14 +2031,14 @@
         <v>14</v>
       </c>
       <c r="F29" s="16"/>
-      <c r="G29" s="48"/>
+      <c r="G29" s="49"/>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
       <c r="J29" s="24"/>
       <c r="K29" s="18"/>
       <c r="L29" s="26"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="49"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
       <c r="O29" s="24"/>
       <c r="P29" s="24"/>
       <c r="Q29" s="24"/>
@@ -2140,7 +2140,7 @@
       <c r="Q32" s="14"/>
       <c r="R32" s="14"/>
       <c r="S32" s="14"/>
-      <c r="T32" s="50"/>
+      <c r="T32" s="51"/>
       <c r="U32" s="14"/>
       <c r="V32" s="14"/>
     </row>
@@ -2172,7 +2172,7 @@
       <c r="Q33" s="14"/>
       <c r="R33" s="14"/>
       <c r="S33" s="14"/>
-      <c r="T33" s="50"/>
+      <c r="T33" s="51"/>
       <c r="U33" s="14"/>
       <c r="V33" s="14"/>
     </row>
@@ -2183,7 +2183,7 @@
       <c r="B34" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="C34" s="51" t="s">
+      <c r="C34" s="48" t="s">
         <v>53</v>
       </c>
       <c r="D34" s="16"/>
@@ -2250,10 +2250,10 @@
       <c r="A36" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="45" t="n">
+      <c r="B36" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="48" t="s">
         <v>57</v>
       </c>
       <c r="D36" s="16" t="s">
@@ -2282,7 +2282,7 @@
       <c r="S36" s="54"/>
       <c r="T36" s="54"/>
       <c r="U36" s="54"/>
-      <c r="V36" s="45"/>
+      <c r="V36" s="46"/>
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="25" t="s">
@@ -2342,9 +2342,9 @@
       <c r="O38" s="19"/>
       <c r="P38" s="19"/>
       <c r="Q38" s="19"/>
-      <c r="R38" s="43"/>
-      <c r="S38" s="43"/>
-      <c r="T38" s="43"/>
+      <c r="R38" s="44"/>
+      <c r="S38" s="44"/>
+      <c r="T38" s="44"/>
       <c r="U38" s="18"/>
       <c r="V38" s="14"/>
     </row>
@@ -2352,7 +2352,7 @@
       <c r="A39" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="45" t="n">
+      <c r="B39" s="46" t="n">
         <v>1</v>
       </c>
       <c r="C39" s="15" t="s">
@@ -2390,7 +2390,7 @@
       <c r="A40" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="45" t="n">
+      <c r="B40" s="46" t="n">
         <v>1</v>
       </c>
       <c r="C40" s="15" t="s">

</xml_diff>

<commit_message>
Toda la funcionalidad terminada faltan cositas
</commit_message>
<xml_diff>
--- a/seed-src/Reuniones de seguimiento y Cronograma/Cronograma I3 Grupo B.xlsx
+++ b/seed-src/Reuniones de seguimiento y Cronograma/Cronograma I3 Grupo B.xlsx
@@ -1077,8 +1077,8 @@
   </sheetPr>
   <dimension ref="A1:X47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2253,7 +2253,7 @@
       <c r="B36" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="C36" s="51" t="s">
+      <c r="C36" s="21" t="s">
         <v>57</v>
       </c>
       <c r="D36" s="16" t="s">

</xml_diff>